<commit_message>
edited the control unit
</commit_message>
<xml_diff>
--- a/Instruction_Bit_Details_Incomplete.xlsx
+++ b/Instruction_Bit_Details_Incomplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University_courses\Senior_1\Spring_2022\architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA374447-5D4D-4B4E-8F24-B426DFCA0944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744381FF-D8F6-476B-88DC-76C14073260F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="602" activeTab="2" xr2:uid="{21FFFC0F-160C-4067-BA4B-4B2E8B2D0BFE}"/>
   </bookViews>
@@ -1062,84 +1062,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1147,6 +1069,84 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1491,48 +1491,48 @@
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="52" t="s">
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
-      <c r="AM2" s="53"/>
-      <c r="AN2" s="53"/>
-      <c r="AO2" s="54"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="59"/>
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="59"/>
+      <c r="AH2" s="59"/>
+      <c r="AI2" s="59"/>
+      <c r="AJ2" s="59"/>
+      <c r="AK2" s="59"/>
+      <c r="AL2" s="59"/>
+      <c r="AM2" s="59"/>
+      <c r="AN2" s="59"/>
+      <c r="AO2" s="60"/>
     </row>
     <row r="3" spans="2:41" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3">
@@ -3227,48 +3227,48 @@
       <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="52" t="s">
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="53"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="53"/>
-      <c r="AB3" s="53"/>
-      <c r="AC3" s="53"/>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53"/>
-      <c r="AJ3" s="53"/>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="53"/>
-      <c r="AM3" s="53"/>
-      <c r="AN3" s="53"/>
-      <c r="AO3" s="53"/>
-      <c r="AP3" s="53"/>
-      <c r="AQ3" s="53"/>
-      <c r="AR3" s="53"/>
-      <c r="AS3" s="53"/>
-      <c r="AT3" s="54"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="59"/>
+      <c r="AG3" s="59"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="59"/>
+      <c r="AJ3" s="59"/>
+      <c r="AK3" s="59"/>
+      <c r="AL3" s="59"/>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="59"/>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="59"/>
+      <c r="AQ3" s="59"/>
+      <c r="AR3" s="59"/>
+      <c r="AS3" s="59"/>
+      <c r="AT3" s="60"/>
       <c r="AU3" s="1" t="s">
         <v>37</v>
       </c>
@@ -3306,43 +3306,43 @@
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
       <c r="M4" s="23"/>
-      <c r="N4" s="55" t="s">
+      <c r="N4" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="64" t="s">
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="64"/>
-      <c r="AA4" s="64"/>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="64"/>
-      <c r="AD4" s="64"/>
-      <c r="AE4" s="64"/>
-      <c r="AF4" s="64"/>
-      <c r="AG4" s="64"/>
-      <c r="AH4" s="64"/>
-      <c r="AI4" s="64"/>
-      <c r="AJ4" s="64"/>
-      <c r="AK4" s="64"/>
-      <c r="AL4" s="64"/>
-      <c r="AM4" s="64"/>
-      <c r="AN4" s="64"/>
-      <c r="AO4" s="64"/>
-      <c r="AP4" s="64"/>
-      <c r="AQ4" s="64"/>
-      <c r="AR4" s="64"/>
-      <c r="AS4" s="64"/>
-      <c r="AT4" s="64"/>
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="79"/>
+      <c r="Z4" s="79"/>
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="79"/>
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="79"/>
+      <c r="AN4" s="79"/>
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="79"/>
       <c r="AU4" s="28" t="s">
         <v>38</v>
       </c>
@@ -3378,41 +3378,41 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="18"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="65" t="s">
+      <c r="N5" s="73"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="65"/>
-      <c r="Z5" s="65"/>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="65"/>
-      <c r="AC5" s="65"/>
-      <c r="AD5" s="65"/>
-      <c r="AE5" s="65"/>
-      <c r="AF5" s="65"/>
-      <c r="AG5" s="65"/>
-      <c r="AH5" s="65"/>
-      <c r="AI5" s="65"/>
-      <c r="AJ5" s="65"/>
-      <c r="AK5" s="65"/>
-      <c r="AL5" s="65"/>
-      <c r="AM5" s="65"/>
-      <c r="AN5" s="65"/>
-      <c r="AO5" s="65"/>
-      <c r="AP5" s="65"/>
-      <c r="AQ5" s="65"/>
-      <c r="AR5" s="65"/>
-      <c r="AS5" s="65"/>
-      <c r="AT5" s="65"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="61"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="61"/>
+      <c r="X5" s="61"/>
+      <c r="Y5" s="61"/>
+      <c r="Z5" s="61"/>
+      <c r="AA5" s="61"/>
+      <c r="AB5" s="61"/>
+      <c r="AC5" s="61"/>
+      <c r="AD5" s="61"/>
+      <c r="AE5" s="61"/>
+      <c r="AF5" s="61"/>
+      <c r="AG5" s="61"/>
+      <c r="AH5" s="61"/>
+      <c r="AI5" s="61"/>
+      <c r="AJ5" s="61"/>
+      <c r="AK5" s="61"/>
+      <c r="AL5" s="61"/>
+      <c r="AM5" s="61"/>
+      <c r="AN5" s="61"/>
+      <c r="AO5" s="61"/>
+      <c r="AP5" s="61"/>
+      <c r="AQ5" s="61"/>
+      <c r="AR5" s="61"/>
+      <c r="AS5" s="61"/>
+      <c r="AT5" s="61"/>
       <c r="AU5" s="29" t="s">
         <v>39</v>
       </c>
@@ -3448,11 +3448,11 @@
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="60"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="75"/>
       <c r="S6" s="66" t="s">
         <v>36</v>
       </c>
@@ -3514,41 +3514,41 @@
         <v>11</v>
       </c>
       <c r="M7" s="26"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="60"/>
-      <c r="S7" s="72"/>
-      <c r="T7" s="65"/>
-      <c r="U7" s="65"/>
-      <c r="V7" s="65"/>
-      <c r="W7" s="65"/>
-      <c r="X7" s="65"/>
-      <c r="Y7" s="65"/>
-      <c r="Z7" s="65"/>
-      <c r="AA7" s="65"/>
-      <c r="AB7" s="65"/>
-      <c r="AC7" s="65"/>
-      <c r="AD7" s="65"/>
-      <c r="AE7" s="72" t="s">
+      <c r="N7" s="73"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="61"/>
+      <c r="U7" s="61"/>
+      <c r="V7" s="61"/>
+      <c r="W7" s="61"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="61"/>
+      <c r="Z7" s="61"/>
+      <c r="AA7" s="61"/>
+      <c r="AB7" s="61"/>
+      <c r="AC7" s="61"/>
+      <c r="AD7" s="61"/>
+      <c r="AE7" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="AF7" s="65"/>
-      <c r="AG7" s="65"/>
-      <c r="AH7" s="65"/>
-      <c r="AI7" s="65"/>
-      <c r="AJ7" s="65"/>
-      <c r="AK7" s="65"/>
-      <c r="AL7" s="65"/>
-      <c r="AM7" s="65"/>
-      <c r="AN7" s="65"/>
-      <c r="AO7" s="65"/>
-      <c r="AP7" s="65"/>
-      <c r="AQ7" s="65"/>
-      <c r="AR7" s="65"/>
-      <c r="AS7" s="65"/>
-      <c r="AT7" s="73"/>
+      <c r="AF7" s="61"/>
+      <c r="AG7" s="61"/>
+      <c r="AH7" s="61"/>
+      <c r="AI7" s="61"/>
+      <c r="AJ7" s="61"/>
+      <c r="AK7" s="61"/>
+      <c r="AL7" s="61"/>
+      <c r="AM7" s="61"/>
+      <c r="AN7" s="61"/>
+      <c r="AO7" s="61"/>
+      <c r="AP7" s="61"/>
+      <c r="AQ7" s="61"/>
+      <c r="AR7" s="61"/>
+      <c r="AS7" s="61"/>
+      <c r="AT7" s="64"/>
       <c r="AU7" s="31" t="s">
         <v>57</v>
       </c>
@@ -3580,11 +3580,11 @@
         <v>11</v>
       </c>
       <c r="M8" s="15"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="59"/>
-      <c r="R8" s="60"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="75"/>
       <c r="S8" s="66"/>
       <c r="T8" s="66"/>
       <c r="U8" s="67"/>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="W8" s="66"/>
       <c r="X8" s="67"/>
-      <c r="Y8" s="69"/>
+      <c r="Y8" s="68"/>
       <c r="Z8" s="66"/>
       <c r="AA8" s="66"/>
       <c r="AB8" s="66"/>
@@ -3614,7 +3614,7 @@
       <c r="AQ8" s="66"/>
       <c r="AR8" s="66"/>
       <c r="AS8" s="66"/>
-      <c r="AT8" s="70"/>
+      <c r="AT8" s="69"/>
       <c r="AU8" s="30" t="s">
         <v>43</v>
       </c>
@@ -3650,41 +3650,41 @@
       <c r="M9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="58"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="65" t="s">
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="T9" s="65"/>
-      <c r="U9" s="68"/>
-      <c r="V9" s="72"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="65"/>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="65"/>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="65"/>
-      <c r="AD9" s="65"/>
-      <c r="AE9" s="65"/>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="65"/>
-      <c r="AH9" s="65"/>
-      <c r="AI9" s="65"/>
-      <c r="AJ9" s="65"/>
-      <c r="AK9" s="65"/>
-      <c r="AL9" s="65"/>
-      <c r="AM9" s="65"/>
-      <c r="AN9" s="65"/>
-      <c r="AO9" s="65"/>
-      <c r="AP9" s="65"/>
-      <c r="AQ9" s="65"/>
-      <c r="AR9" s="65"/>
-      <c r="AS9" s="65"/>
-      <c r="AT9" s="73"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="61"/>
+      <c r="AB9" s="61"/>
+      <c r="AC9" s="61"/>
+      <c r="AD9" s="61"/>
+      <c r="AE9" s="61"/>
+      <c r="AF9" s="61"/>
+      <c r="AG9" s="61"/>
+      <c r="AH9" s="61"/>
+      <c r="AI9" s="61"/>
+      <c r="AJ9" s="61"/>
+      <c r="AK9" s="61"/>
+      <c r="AL9" s="61"/>
+      <c r="AM9" s="61"/>
+      <c r="AN9" s="61"/>
+      <c r="AO9" s="61"/>
+      <c r="AP9" s="61"/>
+      <c r="AQ9" s="61"/>
+      <c r="AR9" s="61"/>
+      <c r="AS9" s="61"/>
+      <c r="AT9" s="64"/>
       <c r="AU9" s="29" t="s">
         <v>45</v>
       </c>
@@ -3717,11 +3717,11 @@
         <v>11</v>
       </c>
       <c r="M10" s="15"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="60"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="75"/>
       <c r="S10" s="66" t="s">
         <v>36</v>
       </c>
@@ -3783,41 +3783,41 @@
         <v>11</v>
       </c>
       <c r="M11" s="22"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="59"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="65" t="s">
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="65"/>
-      <c r="X11" s="65"/>
-      <c r="Y11" s="65"/>
-      <c r="Z11" s="65"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="65"/>
-      <c r="AD11" s="65"/>
-      <c r="AE11" s="65"/>
-      <c r="AF11" s="65"/>
-      <c r="AG11" s="65"/>
-      <c r="AH11" s="65"/>
-      <c r="AI11" s="65"/>
-      <c r="AJ11" s="65"/>
-      <c r="AK11" s="65"/>
-      <c r="AL11" s="65"/>
-      <c r="AM11" s="65"/>
-      <c r="AN11" s="65"/>
-      <c r="AO11" s="65"/>
-      <c r="AP11" s="65"/>
-      <c r="AQ11" s="65"/>
-      <c r="AR11" s="65"/>
-      <c r="AS11" s="65"/>
-      <c r="AT11" s="65"/>
+      <c r="T11" s="61"/>
+      <c r="U11" s="61"/>
+      <c r="V11" s="61"/>
+      <c r="W11" s="61"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="61"/>
+      <c r="Z11" s="61"/>
+      <c r="AA11" s="61"/>
+      <c r="AB11" s="61"/>
+      <c r="AC11" s="61"/>
+      <c r="AD11" s="61"/>
+      <c r="AE11" s="61"/>
+      <c r="AF11" s="61"/>
+      <c r="AG11" s="61"/>
+      <c r="AH11" s="61"/>
+      <c r="AI11" s="61"/>
+      <c r="AJ11" s="61"/>
+      <c r="AK11" s="61"/>
+      <c r="AL11" s="61"/>
+      <c r="AM11" s="61"/>
+      <c r="AN11" s="61"/>
+      <c r="AO11" s="61"/>
+      <c r="AP11" s="61"/>
+      <c r="AQ11" s="61"/>
+      <c r="AR11" s="61"/>
+      <c r="AS11" s="61"/>
+      <c r="AT11" s="61"/>
       <c r="AU11" s="29" t="s">
         <v>47</v>
       </c>
@@ -3850,15 +3850,15 @@
         <v>11</v>
       </c>
       <c r="M12" s="21"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="60"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="75"/>
       <c r="S12" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="T12" s="69"/>
+      <c r="T12" s="68"/>
       <c r="U12" s="66"/>
       <c r="V12" s="66"/>
       <c r="W12" s="66"/>
@@ -3884,7 +3884,7 @@
       <c r="AQ12" s="66"/>
       <c r="AR12" s="66"/>
       <c r="AS12" s="66"/>
-      <c r="AT12" s="70"/>
+      <c r="AT12" s="69"/>
       <c r="AU12" s="30" t="s">
         <v>51</v>
       </c>
@@ -3914,41 +3914,41 @@
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="65"/>
-      <c r="T13" s="65"/>
-      <c r="U13" s="68"/>
-      <c r="V13" s="65" t="s">
+      <c r="N13" s="73"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="75"/>
+      <c r="S13" s="61"/>
+      <c r="T13" s="61"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="W13" s="65"/>
-      <c r="X13" s="68"/>
-      <c r="Y13" s="72"/>
-      <c r="Z13" s="65"/>
-      <c r="AA13" s="65"/>
-      <c r="AB13" s="65"/>
-      <c r="AC13" s="65"/>
-      <c r="AD13" s="65"/>
-      <c r="AE13" s="65"/>
-      <c r="AF13" s="65"/>
-      <c r="AG13" s="65"/>
-      <c r="AH13" s="65"/>
-      <c r="AI13" s="65"/>
-      <c r="AJ13" s="65"/>
-      <c r="AK13" s="65"/>
-      <c r="AL13" s="65"/>
-      <c r="AM13" s="65"/>
-      <c r="AN13" s="65"/>
-      <c r="AO13" s="65"/>
-      <c r="AP13" s="65"/>
-      <c r="AQ13" s="65"/>
-      <c r="AR13" s="65"/>
-      <c r="AS13" s="65"/>
-      <c r="AT13" s="73"/>
+      <c r="W13" s="61"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="63"/>
+      <c r="Z13" s="61"/>
+      <c r="AA13" s="61"/>
+      <c r="AB13" s="61"/>
+      <c r="AC13" s="61"/>
+      <c r="AD13" s="61"/>
+      <c r="AE13" s="61"/>
+      <c r="AF13" s="61"/>
+      <c r="AG13" s="61"/>
+      <c r="AH13" s="61"/>
+      <c r="AI13" s="61"/>
+      <c r="AJ13" s="61"/>
+      <c r="AK13" s="61"/>
+      <c r="AL13" s="61"/>
+      <c r="AM13" s="61"/>
+      <c r="AN13" s="61"/>
+      <c r="AO13" s="61"/>
+      <c r="AP13" s="61"/>
+      <c r="AQ13" s="61"/>
+      <c r="AR13" s="61"/>
+      <c r="AS13" s="61"/>
+      <c r="AT13" s="64"/>
       <c r="AU13" s="29" t="s">
         <v>50</v>
       </c>
@@ -3980,17 +3980,17 @@
       <c r="M14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="58"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="59"/>
-      <c r="R14" s="60"/>
+      <c r="N14" s="73"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="74"/>
+      <c r="Q14" s="74"/>
+      <c r="R14" s="75"/>
       <c r="S14" s="66" t="s">
         <v>44</v>
       </c>
       <c r="T14" s="66"/>
       <c r="U14" s="67"/>
-      <c r="V14" s="69"/>
+      <c r="V14" s="68"/>
       <c r="W14" s="66"/>
       <c r="X14" s="66"/>
       <c r="Y14" s="66"/>
@@ -4014,7 +4014,7 @@
       <c r="AQ14" s="66"/>
       <c r="AR14" s="66"/>
       <c r="AS14" s="66"/>
-      <c r="AT14" s="70"/>
+      <c r="AT14" s="69"/>
       <c r="AU14" s="31" t="s">
         <v>52</v>
       </c>
@@ -4046,43 +4046,43 @@
       <c r="M15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="58"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="65" t="s">
+      <c r="N15" s="73"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="75"/>
+      <c r="S15" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="T15" s="65"/>
-      <c r="U15" s="68"/>
-      <c r="V15" s="72" t="s">
+      <c r="T15" s="61"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="W15" s="65"/>
-      <c r="X15" s="68"/>
-      <c r="Y15" s="72"/>
-      <c r="Z15" s="65"/>
-      <c r="AA15" s="65"/>
-      <c r="AB15" s="65"/>
-      <c r="AC15" s="65"/>
-      <c r="AD15" s="65"/>
-      <c r="AE15" s="65"/>
-      <c r="AF15" s="65"/>
-      <c r="AG15" s="65"/>
-      <c r="AH15" s="65"/>
-      <c r="AI15" s="65"/>
-      <c r="AJ15" s="65"/>
-      <c r="AK15" s="65"/>
-      <c r="AL15" s="65"/>
-      <c r="AM15" s="65"/>
-      <c r="AN15" s="65"/>
-      <c r="AO15" s="65"/>
-      <c r="AP15" s="65"/>
-      <c r="AQ15" s="65"/>
-      <c r="AR15" s="65"/>
-      <c r="AS15" s="65"/>
-      <c r="AT15" s="73"/>
+      <c r="W15" s="61"/>
+      <c r="X15" s="62"/>
+      <c r="Y15" s="63"/>
+      <c r="Z15" s="61"/>
+      <c r="AA15" s="61"/>
+      <c r="AB15" s="61"/>
+      <c r="AC15" s="61"/>
+      <c r="AD15" s="61"/>
+      <c r="AE15" s="61"/>
+      <c r="AF15" s="61"/>
+      <c r="AG15" s="61"/>
+      <c r="AH15" s="61"/>
+      <c r="AI15" s="61"/>
+      <c r="AJ15" s="61"/>
+      <c r="AK15" s="61"/>
+      <c r="AL15" s="61"/>
+      <c r="AM15" s="61"/>
+      <c r="AN15" s="61"/>
+      <c r="AO15" s="61"/>
+      <c r="AP15" s="61"/>
+      <c r="AQ15" s="61"/>
+      <c r="AR15" s="61"/>
+      <c r="AS15" s="61"/>
+      <c r="AT15" s="64"/>
       <c r="AU15" s="29" t="s">
         <v>53</v>
       </c>
@@ -4120,17 +4120,17 @@
       <c r="M16" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="58"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="59"/>
-      <c r="R16" s="60"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74"/>
+      <c r="Q16" s="74"/>
+      <c r="R16" s="75"/>
       <c r="S16" s="66" t="s">
         <v>44</v>
       </c>
       <c r="T16" s="66"/>
       <c r="U16" s="67"/>
-      <c r="V16" s="69"/>
+      <c r="V16" s="68"/>
       <c r="W16" s="66"/>
       <c r="X16" s="66"/>
       <c r="Y16" s="66"/>
@@ -4139,7 +4139,7 @@
       <c r="AB16" s="66"/>
       <c r="AC16" s="66"/>
       <c r="AD16" s="67"/>
-      <c r="AE16" s="69" t="s">
+      <c r="AE16" s="68" t="s">
         <v>41</v>
       </c>
       <c r="AF16" s="66"/>
@@ -4156,7 +4156,7 @@
       <c r="AQ16" s="66"/>
       <c r="AR16" s="66"/>
       <c r="AS16" s="66"/>
-      <c r="AT16" s="70"/>
+      <c r="AT16" s="69"/>
       <c r="AU16" s="31" t="s">
         <v>55</v>
       </c>
@@ -4188,43 +4188,43 @@
       <c r="M17" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="N17" s="58"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="60"/>
-      <c r="S17" s="65" t="s">
+      <c r="N17" s="73"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="T17" s="65"/>
-      <c r="U17" s="68"/>
-      <c r="V17" s="72" t="s">
+      <c r="T17" s="61"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="W17" s="65"/>
-      <c r="X17" s="68"/>
-      <c r="Y17" s="72"/>
-      <c r="Z17" s="65"/>
-      <c r="AA17" s="65"/>
-      <c r="AB17" s="65"/>
-      <c r="AC17" s="65"/>
-      <c r="AD17" s="65"/>
-      <c r="AE17" s="65"/>
-      <c r="AF17" s="65"/>
-      <c r="AG17" s="65"/>
-      <c r="AH17" s="65"/>
-      <c r="AI17" s="65"/>
-      <c r="AJ17" s="65"/>
-      <c r="AK17" s="65"/>
-      <c r="AL17" s="65"/>
-      <c r="AM17" s="65"/>
-      <c r="AN17" s="65"/>
-      <c r="AO17" s="65"/>
-      <c r="AP17" s="65"/>
-      <c r="AQ17" s="65"/>
-      <c r="AR17" s="65"/>
-      <c r="AS17" s="65"/>
-      <c r="AT17" s="73"/>
+      <c r="W17" s="61"/>
+      <c r="X17" s="62"/>
+      <c r="Y17" s="63"/>
+      <c r="Z17" s="61"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="61"/>
+      <c r="AF17" s="61"/>
+      <c r="AG17" s="61"/>
+      <c r="AH17" s="61"/>
+      <c r="AI17" s="61"/>
+      <c r="AJ17" s="61"/>
+      <c r="AK17" s="61"/>
+      <c r="AL17" s="61"/>
+      <c r="AM17" s="61"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="61"/>
+      <c r="AP17" s="61"/>
+      <c r="AQ17" s="61"/>
+      <c r="AR17" s="61"/>
+      <c r="AS17" s="61"/>
+      <c r="AT17" s="64"/>
       <c r="AU17" s="34" t="s">
         <v>56</v>
       </c>
@@ -4258,12 +4258,12 @@
       <c r="K18" s="27"/>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="60"/>
-      <c r="S18" s="71"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="74"/>
+      <c r="P18" s="74"/>
+      <c r="Q18" s="74"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="65"/>
       <c r="T18" s="66"/>
       <c r="U18" s="66"/>
       <c r="V18" s="66"/>
@@ -4275,7 +4275,7 @@
       <c r="AB18" s="66"/>
       <c r="AC18" s="66"/>
       <c r="AD18" s="67"/>
-      <c r="AE18" s="69" t="s">
+      <c r="AE18" s="68" t="s">
         <v>41</v>
       </c>
       <c r="AF18" s="66"/>
@@ -4292,7 +4292,7 @@
       <c r="AQ18" s="66"/>
       <c r="AR18" s="66"/>
       <c r="AS18" s="66"/>
-      <c r="AT18" s="70"/>
+      <c r="AT18" s="69"/>
       <c r="AU18" s="29" t="s">
         <v>42</v>
       </c>
@@ -4326,41 +4326,41 @@
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
       <c r="M19" s="18"/>
-      <c r="N19" s="58"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="60"/>
-      <c r="S19" s="72"/>
-      <c r="T19" s="65"/>
-      <c r="U19" s="65"/>
-      <c r="V19" s="65"/>
-      <c r="W19" s="65"/>
-      <c r="X19" s="65"/>
-      <c r="Y19" s="65"/>
-      <c r="Z19" s="65"/>
-      <c r="AA19" s="65"/>
-      <c r="AB19" s="65"/>
-      <c r="AC19" s="65"/>
-      <c r="AD19" s="65"/>
-      <c r="AE19" s="72" t="s">
+      <c r="N19" s="73"/>
+      <c r="O19" s="74"/>
+      <c r="P19" s="74"/>
+      <c r="Q19" s="74"/>
+      <c r="R19" s="75"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="61"/>
+      <c r="U19" s="61"/>
+      <c r="V19" s="61"/>
+      <c r="W19" s="61"/>
+      <c r="X19" s="61"/>
+      <c r="Y19" s="61"/>
+      <c r="Z19" s="61"/>
+      <c r="AA19" s="61"/>
+      <c r="AB19" s="61"/>
+      <c r="AC19" s="61"/>
+      <c r="AD19" s="61"/>
+      <c r="AE19" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="AF19" s="65"/>
-      <c r="AG19" s="65"/>
-      <c r="AH19" s="65"/>
-      <c r="AI19" s="65"/>
-      <c r="AJ19" s="65"/>
-      <c r="AK19" s="65"/>
-      <c r="AL19" s="65"/>
-      <c r="AM19" s="65"/>
-      <c r="AN19" s="65"/>
-      <c r="AO19" s="65"/>
-      <c r="AP19" s="65"/>
-      <c r="AQ19" s="65"/>
-      <c r="AR19" s="65"/>
-      <c r="AS19" s="65"/>
-      <c r="AT19" s="73"/>
+      <c r="AF19" s="61"/>
+      <c r="AG19" s="61"/>
+      <c r="AH19" s="61"/>
+      <c r="AI19" s="61"/>
+      <c r="AJ19" s="61"/>
+      <c r="AK19" s="61"/>
+      <c r="AL19" s="61"/>
+      <c r="AM19" s="61"/>
+      <c r="AN19" s="61"/>
+      <c r="AO19" s="61"/>
+      <c r="AP19" s="61"/>
+      <c r="AQ19" s="61"/>
+      <c r="AR19" s="61"/>
+      <c r="AS19" s="61"/>
+      <c r="AT19" s="64"/>
       <c r="AU19" s="29" t="s">
         <v>58</v>
       </c>
@@ -4394,12 +4394,12 @@
       <c r="K20" s="13"/>
       <c r="L20" s="14"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="59"/>
-      <c r="R20" s="60"/>
-      <c r="S20" s="71"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="74"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="75"/>
+      <c r="S20" s="65"/>
       <c r="T20" s="66"/>
       <c r="U20" s="66"/>
       <c r="V20" s="66"/>
@@ -4411,7 +4411,7 @@
       <c r="AB20" s="66"/>
       <c r="AC20" s="66"/>
       <c r="AD20" s="67"/>
-      <c r="AE20" s="69" t="s">
+      <c r="AE20" s="68" t="s">
         <v>41</v>
       </c>
       <c r="AF20" s="66"/>
@@ -4428,7 +4428,7 @@
       <c r="AQ20" s="66"/>
       <c r="AR20" s="66"/>
       <c r="AS20" s="66"/>
-      <c r="AT20" s="70"/>
+      <c r="AT20" s="69"/>
       <c r="AU20" s="30" t="s">
         <v>59</v>
       </c>
@@ -4462,41 +4462,41 @@
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
       <c r="M21" s="18"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="59"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="72"/>
-      <c r="T21" s="65"/>
-      <c r="U21" s="65"/>
-      <c r="V21" s="65"/>
-      <c r="W21" s="65"/>
-      <c r="X21" s="65"/>
-      <c r="Y21" s="65"/>
-      <c r="Z21" s="65"/>
-      <c r="AA21" s="65"/>
-      <c r="AB21" s="65"/>
-      <c r="AC21" s="65"/>
-      <c r="AD21" s="65"/>
-      <c r="AE21" s="72" t="s">
+      <c r="N21" s="73"/>
+      <c r="O21" s="74"/>
+      <c r="P21" s="74"/>
+      <c r="Q21" s="74"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="63"/>
+      <c r="T21" s="61"/>
+      <c r="U21" s="61"/>
+      <c r="V21" s="61"/>
+      <c r="W21" s="61"/>
+      <c r="X21" s="61"/>
+      <c r="Y21" s="61"/>
+      <c r="Z21" s="61"/>
+      <c r="AA21" s="61"/>
+      <c r="AB21" s="61"/>
+      <c r="AC21" s="61"/>
+      <c r="AD21" s="61"/>
+      <c r="AE21" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="AF21" s="65"/>
-      <c r="AG21" s="65"/>
-      <c r="AH21" s="65"/>
-      <c r="AI21" s="65"/>
-      <c r="AJ21" s="65"/>
-      <c r="AK21" s="65"/>
-      <c r="AL21" s="65"/>
-      <c r="AM21" s="65"/>
-      <c r="AN21" s="65"/>
-      <c r="AO21" s="65"/>
-      <c r="AP21" s="65"/>
-      <c r="AQ21" s="65"/>
-      <c r="AR21" s="65"/>
-      <c r="AS21" s="65"/>
-      <c r="AT21" s="73"/>
+      <c r="AF21" s="61"/>
+      <c r="AG21" s="61"/>
+      <c r="AH21" s="61"/>
+      <c r="AI21" s="61"/>
+      <c r="AJ21" s="61"/>
+      <c r="AK21" s="61"/>
+      <c r="AL21" s="61"/>
+      <c r="AM21" s="61"/>
+      <c r="AN21" s="61"/>
+      <c r="AO21" s="61"/>
+      <c r="AP21" s="61"/>
+      <c r="AQ21" s="61"/>
+      <c r="AR21" s="61"/>
+      <c r="AS21" s="61"/>
+      <c r="AT21" s="64"/>
       <c r="AU21" s="29" t="s">
         <v>60</v>
       </c>
@@ -4532,11 +4532,11 @@
         <v>11</v>
       </c>
       <c r="M22" s="15"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="60"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="75"/>
       <c r="S22" s="66"/>
       <c r="T22" s="66"/>
       <c r="U22" s="67"/>
@@ -4550,10 +4550,10 @@
       </c>
       <c r="Z22" s="66"/>
       <c r="AA22" s="67"/>
-      <c r="AB22" s="69"/>
+      <c r="AB22" s="68"/>
       <c r="AC22" s="66"/>
       <c r="AD22" s="67"/>
-      <c r="AE22" s="69" t="s">
+      <c r="AE22" s="68" t="s">
         <v>41</v>
       </c>
       <c r="AF22" s="66"/>
@@ -4570,7 +4570,7 @@
       <c r="AQ22" s="66"/>
       <c r="AR22" s="66"/>
       <c r="AS22" s="66"/>
-      <c r="AT22" s="70"/>
+      <c r="AT22" s="69"/>
       <c r="AU22" s="30" t="s">
         <v>70</v>
       </c>
@@ -4606,43 +4606,43 @@
       <c r="M23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N23" s="58"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="65" t="s">
+      <c r="N23" s="73"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="T23" s="65"/>
-      <c r="U23" s="68"/>
-      <c r="V23" s="72" t="s">
+      <c r="T23" s="61"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="W23" s="65"/>
-      <c r="X23" s="68"/>
-      <c r="Y23" s="72"/>
-      <c r="Z23" s="65"/>
-      <c r="AA23" s="65"/>
-      <c r="AB23" s="65"/>
-      <c r="AC23" s="65"/>
-      <c r="AD23" s="65"/>
-      <c r="AE23" s="65"/>
-      <c r="AF23" s="65"/>
-      <c r="AG23" s="65"/>
-      <c r="AH23" s="65"/>
-      <c r="AI23" s="65"/>
-      <c r="AJ23" s="65"/>
-      <c r="AK23" s="65"/>
-      <c r="AL23" s="65"/>
-      <c r="AM23" s="65"/>
-      <c r="AN23" s="65"/>
-      <c r="AO23" s="65"/>
-      <c r="AP23" s="65"/>
-      <c r="AQ23" s="65"/>
-      <c r="AR23" s="65"/>
-      <c r="AS23" s="65"/>
-      <c r="AT23" s="73"/>
+      <c r="W23" s="61"/>
+      <c r="X23" s="62"/>
+      <c r="Y23" s="63"/>
+      <c r="Z23" s="61"/>
+      <c r="AA23" s="61"/>
+      <c r="AB23" s="61"/>
+      <c r="AC23" s="61"/>
+      <c r="AD23" s="61"/>
+      <c r="AE23" s="61"/>
+      <c r="AF23" s="61"/>
+      <c r="AG23" s="61"/>
+      <c r="AH23" s="61"/>
+      <c r="AI23" s="61"/>
+      <c r="AJ23" s="61"/>
+      <c r="AK23" s="61"/>
+      <c r="AL23" s="61"/>
+      <c r="AM23" s="61"/>
+      <c r="AN23" s="61"/>
+      <c r="AO23" s="61"/>
+      <c r="AP23" s="61"/>
+      <c r="AQ23" s="61"/>
+      <c r="AR23" s="61"/>
+      <c r="AS23" s="61"/>
+      <c r="AT23" s="64"/>
       <c r="AU23" s="29" t="s">
         <v>63</v>
       </c>
@@ -4678,12 +4678,12 @@
       <c r="M24" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N24" s="58"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="71" t="s">
+      <c r="N24" s="73"/>
+      <c r="O24" s="74"/>
+      <c r="P24" s="74"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="75"/>
+      <c r="S24" s="65" t="s">
         <v>44</v>
       </c>
       <c r="T24" s="66"/>
@@ -4693,7 +4693,7 @@
       </c>
       <c r="W24" s="66"/>
       <c r="X24" s="67"/>
-      <c r="Y24" s="69"/>
+      <c r="Y24" s="68"/>
       <c r="Z24" s="66"/>
       <c r="AA24" s="66"/>
       <c r="AB24" s="66"/>
@@ -4714,7 +4714,7 @@
       <c r="AQ24" s="66"/>
       <c r="AR24" s="66"/>
       <c r="AS24" s="66"/>
-      <c r="AT24" s="70"/>
+      <c r="AT24" s="69"/>
       <c r="AU24" s="31" t="s">
         <v>64</v>
       </c>
@@ -4750,45 +4750,45 @@
       <c r="M25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N25" s="58"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="65" t="s">
+      <c r="N25" s="73"/>
+      <c r="O25" s="74"/>
+      <c r="P25" s="74"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="75"/>
+      <c r="S25" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="T25" s="65"/>
-      <c r="U25" s="68"/>
-      <c r="V25" s="72" t="s">
+      <c r="T25" s="61"/>
+      <c r="U25" s="62"/>
+      <c r="V25" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="W25" s="65"/>
-      <c r="X25" s="68"/>
-      <c r="Y25" s="72" t="s">
+      <c r="W25" s="61"/>
+      <c r="X25" s="62"/>
+      <c r="Y25" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="Z25" s="65"/>
-      <c r="AA25" s="68"/>
-      <c r="AB25" s="72"/>
-      <c r="AC25" s="65"/>
-      <c r="AD25" s="65"/>
-      <c r="AE25" s="65"/>
-      <c r="AF25" s="65"/>
-      <c r="AG25" s="65"/>
-      <c r="AH25" s="65"/>
-      <c r="AI25" s="65"/>
-      <c r="AJ25" s="65"/>
-      <c r="AK25" s="65"/>
-      <c r="AL25" s="65"/>
-      <c r="AM25" s="65"/>
-      <c r="AN25" s="65"/>
-      <c r="AO25" s="65"/>
-      <c r="AP25" s="65"/>
-      <c r="AQ25" s="65"/>
-      <c r="AR25" s="65"/>
-      <c r="AS25" s="65"/>
-      <c r="AT25" s="73"/>
+      <c r="Z25" s="61"/>
+      <c r="AA25" s="62"/>
+      <c r="AB25" s="63"/>
+      <c r="AC25" s="61"/>
+      <c r="AD25" s="61"/>
+      <c r="AE25" s="61"/>
+      <c r="AF25" s="61"/>
+      <c r="AG25" s="61"/>
+      <c r="AH25" s="61"/>
+      <c r="AI25" s="61"/>
+      <c r="AJ25" s="61"/>
+      <c r="AK25" s="61"/>
+      <c r="AL25" s="61"/>
+      <c r="AM25" s="61"/>
+      <c r="AN25" s="61"/>
+      <c r="AO25" s="61"/>
+      <c r="AP25" s="61"/>
+      <c r="AQ25" s="61"/>
+      <c r="AR25" s="61"/>
+      <c r="AS25" s="61"/>
+      <c r="AT25" s="64"/>
       <c r="AU25" s="29" t="s">
         <v>65</v>
       </c>
@@ -4824,12 +4824,12 @@
       <c r="M26" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N26" s="58"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-      <c r="R26" s="60"/>
-      <c r="S26" s="71" t="s">
+      <c r="N26" s="73"/>
+      <c r="O26" s="74"/>
+      <c r="P26" s="74"/>
+      <c r="Q26" s="74"/>
+      <c r="R26" s="75"/>
+      <c r="S26" s="65" t="s">
         <v>44</v>
       </c>
       <c r="T26" s="66"/>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="Z26" s="66"/>
       <c r="AA26" s="67"/>
-      <c r="AB26" s="69"/>
+      <c r="AB26" s="68"/>
       <c r="AC26" s="66"/>
       <c r="AD26" s="66"/>
       <c r="AE26" s="66"/>
@@ -4862,7 +4862,7 @@
       <c r="AQ26" s="66"/>
       <c r="AR26" s="66"/>
       <c r="AS26" s="66"/>
-      <c r="AT26" s="70"/>
+      <c r="AT26" s="69"/>
       <c r="AU26" s="31" t="s">
         <v>66</v>
       </c>
@@ -4898,45 +4898,45 @@
       <c r="M27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N27" s="58"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="60"/>
-      <c r="S27" s="65" t="s">
+      <c r="N27" s="73"/>
+      <c r="O27" s="74"/>
+      <c r="P27" s="74"/>
+      <c r="Q27" s="74"/>
+      <c r="R27" s="75"/>
+      <c r="S27" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="T27" s="65"/>
-      <c r="U27" s="68"/>
-      <c r="V27" s="72" t="s">
+      <c r="T27" s="61"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="W27" s="65"/>
-      <c r="X27" s="68"/>
-      <c r="Y27" s="72" t="s">
+      <c r="W27" s="61"/>
+      <c r="X27" s="62"/>
+      <c r="Y27" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="Z27" s="65"/>
-      <c r="AA27" s="68"/>
-      <c r="AB27" s="72"/>
-      <c r="AC27" s="65"/>
-      <c r="AD27" s="65"/>
-      <c r="AE27" s="65"/>
-      <c r="AF27" s="65"/>
-      <c r="AG27" s="65"/>
-      <c r="AH27" s="65"/>
-      <c r="AI27" s="65"/>
-      <c r="AJ27" s="65"/>
-      <c r="AK27" s="65"/>
-      <c r="AL27" s="65"/>
-      <c r="AM27" s="65"/>
-      <c r="AN27" s="65"/>
-      <c r="AO27" s="65"/>
-      <c r="AP27" s="65"/>
-      <c r="AQ27" s="65"/>
-      <c r="AR27" s="65"/>
-      <c r="AS27" s="65"/>
-      <c r="AT27" s="73"/>
+      <c r="Z27" s="61"/>
+      <c r="AA27" s="62"/>
+      <c r="AB27" s="63"/>
+      <c r="AC27" s="61"/>
+      <c r="AD27" s="61"/>
+      <c r="AE27" s="61"/>
+      <c r="AF27" s="61"/>
+      <c r="AG27" s="61"/>
+      <c r="AH27" s="61"/>
+      <c r="AI27" s="61"/>
+      <c r="AJ27" s="61"/>
+      <c r="AK27" s="61"/>
+      <c r="AL27" s="61"/>
+      <c r="AM27" s="61"/>
+      <c r="AN27" s="61"/>
+      <c r="AO27" s="61"/>
+      <c r="AP27" s="61"/>
+      <c r="AQ27" s="61"/>
+      <c r="AR27" s="61"/>
+      <c r="AS27" s="61"/>
+      <c r="AT27" s="64"/>
       <c r="AU27" s="29" t="s">
         <v>67</v>
       </c>
@@ -4972,12 +4972,12 @@
       <c r="M28" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N28" s="58"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="71" t="s">
+      <c r="N28" s="73"/>
+      <c r="O28" s="74"/>
+      <c r="P28" s="74"/>
+      <c r="Q28" s="74"/>
+      <c r="R28" s="75"/>
+      <c r="S28" s="65" t="s">
         <v>44</v>
       </c>
       <c r="T28" s="66"/>
@@ -4987,13 +4987,13 @@
       </c>
       <c r="W28" s="66"/>
       <c r="X28" s="67"/>
-      <c r="Y28" s="69"/>
+      <c r="Y28" s="68"/>
       <c r="Z28" s="66"/>
       <c r="AA28" s="66"/>
       <c r="AB28" s="66"/>
       <c r="AC28" s="66"/>
       <c r="AD28" s="67"/>
-      <c r="AE28" s="69" t="s">
+      <c r="AE28" s="68" t="s">
         <v>41</v>
       </c>
       <c r="AF28" s="66"/>
@@ -5010,7 +5010,7 @@
       <c r="AQ28" s="66"/>
       <c r="AR28" s="66"/>
       <c r="AS28" s="66"/>
-      <c r="AT28" s="70"/>
+      <c r="AT28" s="69"/>
       <c r="AU28" s="31" t="s">
         <v>68</v>
       </c>
@@ -5050,45 +5050,45 @@
       <c r="M29" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N29" s="58"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
-      <c r="R29" s="60"/>
-      <c r="S29" s="65" t="s">
+      <c r="N29" s="73"/>
+      <c r="O29" s="74"/>
+      <c r="P29" s="74"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="75"/>
+      <c r="S29" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="T29" s="65"/>
-      <c r="U29" s="68"/>
-      <c r="V29" s="72" t="s">
+      <c r="T29" s="61"/>
+      <c r="U29" s="62"/>
+      <c r="V29" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="W29" s="65"/>
-      <c r="X29" s="68"/>
-      <c r="Y29" s="72"/>
-      <c r="Z29" s="65"/>
-      <c r="AA29" s="65"/>
-      <c r="AB29" s="65"/>
-      <c r="AC29" s="65"/>
-      <c r="AD29" s="68"/>
-      <c r="AE29" s="72" t="s">
+      <c r="W29" s="61"/>
+      <c r="X29" s="62"/>
+      <c r="Y29" s="63"/>
+      <c r="Z29" s="61"/>
+      <c r="AA29" s="61"/>
+      <c r="AB29" s="61"/>
+      <c r="AC29" s="61"/>
+      <c r="AD29" s="62"/>
+      <c r="AE29" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="AF29" s="65"/>
-      <c r="AG29" s="65"/>
-      <c r="AH29" s="65"/>
-      <c r="AI29" s="65"/>
-      <c r="AJ29" s="65"/>
-      <c r="AK29" s="65"/>
-      <c r="AL29" s="65"/>
-      <c r="AM29" s="65"/>
-      <c r="AN29" s="65"/>
-      <c r="AO29" s="65"/>
-      <c r="AP29" s="65"/>
-      <c r="AQ29" s="65"/>
-      <c r="AR29" s="65"/>
-      <c r="AS29" s="65"/>
-      <c r="AT29" s="73"/>
+      <c r="AF29" s="61"/>
+      <c r="AG29" s="61"/>
+      <c r="AH29" s="61"/>
+      <c r="AI29" s="61"/>
+      <c r="AJ29" s="61"/>
+      <c r="AK29" s="61"/>
+      <c r="AL29" s="61"/>
+      <c r="AM29" s="61"/>
+      <c r="AN29" s="61"/>
+      <c r="AO29" s="61"/>
+      <c r="AP29" s="61"/>
+      <c r="AQ29" s="61"/>
+      <c r="AR29" s="61"/>
+      <c r="AS29" s="61"/>
+      <c r="AT29" s="64"/>
       <c r="AU29" s="29" t="s">
         <v>69</v>
       </c>
@@ -5108,11 +5108,11 @@
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
       <c r="M30" s="15"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="59"/>
-      <c r="R30" s="60"/>
+      <c r="N30" s="73"/>
+      <c r="O30" s="74"/>
+      <c r="P30" s="74"/>
+      <c r="Q30" s="74"/>
+      <c r="R30" s="75"/>
       <c r="S30" s="14"/>
       <c r="T30" s="14"/>
       <c r="U30" s="14"/>
@@ -5158,11 +5158,11 @@
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
       <c r="M31" s="18"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="59"/>
-      <c r="R31" s="60"/>
+      <c r="N31" s="73"/>
+      <c r="O31" s="74"/>
+      <c r="P31" s="74"/>
+      <c r="Q31" s="74"/>
+      <c r="R31" s="75"/>
       <c r="S31" s="17"/>
       <c r="T31" s="17"/>
       <c r="U31" s="17"/>
@@ -5208,11 +5208,11 @@
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
       <c r="M32" s="15"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="59"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
-      <c r="R32" s="60"/>
+      <c r="N32" s="73"/>
+      <c r="O32" s="74"/>
+      <c r="P32" s="74"/>
+      <c r="Q32" s="74"/>
+      <c r="R32" s="75"/>
       <c r="S32" s="14"/>
       <c r="T32" s="14"/>
       <c r="U32" s="14"/>
@@ -5258,11 +5258,11 @@
       <c r="K33" s="19"/>
       <c r="L33" s="19"/>
       <c r="M33" s="18"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="59"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="59"/>
-      <c r="R33" s="60"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="74"/>
+      <c r="P33" s="74"/>
+      <c r="Q33" s="74"/>
+      <c r="R33" s="75"/>
       <c r="S33" s="17"/>
       <c r="T33" s="17"/>
       <c r="U33" s="17"/>
@@ -5308,11 +5308,11 @@
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="15"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="59"/>
-      <c r="P34" s="59"/>
-      <c r="Q34" s="59"/>
-      <c r="R34" s="60"/>
+      <c r="N34" s="73"/>
+      <c r="O34" s="74"/>
+      <c r="P34" s="74"/>
+      <c r="Q34" s="74"/>
+      <c r="R34" s="75"/>
       <c r="S34" s="14"/>
       <c r="T34" s="14"/>
       <c r="U34" s="14"/>
@@ -5361,11 +5361,11 @@
       <c r="K35" s="37"/>
       <c r="L35" s="37"/>
       <c r="M35" s="38"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="62"/>
-      <c r="P35" s="62"/>
-      <c r="Q35" s="62"/>
-      <c r="R35" s="63"/>
+      <c r="N35" s="76"/>
+      <c r="O35" s="77"/>
+      <c r="P35" s="77"/>
+      <c r="Q35" s="77"/>
+      <c r="R35" s="78"/>
       <c r="S35" s="37"/>
       <c r="T35" s="37"/>
       <c r="U35" s="37"/>
@@ -5399,37 +5399,28 @@
     <row r="36" spans="2:48" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="S29:U29"/>
-    <mergeCell ref="V29:X29"/>
-    <mergeCell ref="AE29:AT29"/>
-    <mergeCell ref="Y29:AD29"/>
-    <mergeCell ref="S27:U27"/>
-    <mergeCell ref="V27:X27"/>
-    <mergeCell ref="Y27:AA27"/>
-    <mergeCell ref="AB27:AT27"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="AE28:AT28"/>
-    <mergeCell ref="Y28:AD28"/>
-    <mergeCell ref="S25:U25"/>
-    <mergeCell ref="V25:X25"/>
-    <mergeCell ref="Y25:AA25"/>
-    <mergeCell ref="AB25:AT25"/>
-    <mergeCell ref="S26:U26"/>
-    <mergeCell ref="V26:X26"/>
-    <mergeCell ref="Y26:AA26"/>
-    <mergeCell ref="AB26:AT26"/>
-    <mergeCell ref="S23:U23"/>
-    <mergeCell ref="V23:X23"/>
-    <mergeCell ref="Y23:AT23"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="V24:X24"/>
-    <mergeCell ref="Y24:AT24"/>
-    <mergeCell ref="S22:U22"/>
-    <mergeCell ref="V22:X22"/>
-    <mergeCell ref="AE22:AT22"/>
-    <mergeCell ref="Y22:AA22"/>
-    <mergeCell ref="AB22:AD22"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:AT3"/>
+    <mergeCell ref="N4:R35"/>
+    <mergeCell ref="S4:AT4"/>
+    <mergeCell ref="S5:AT5"/>
+    <mergeCell ref="S6:AT6"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="AE16:AT16"/>
+    <mergeCell ref="AE18:AT18"/>
+    <mergeCell ref="S18:AD18"/>
+    <mergeCell ref="V9:AT9"/>
+    <mergeCell ref="T12:AT12"/>
+    <mergeCell ref="Y13:AT13"/>
+    <mergeCell ref="V14:AT14"/>
+    <mergeCell ref="S10:AT10"/>
+    <mergeCell ref="S11:AT11"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="V13:X13"/>
     <mergeCell ref="S21:AD21"/>
     <mergeCell ref="AE21:AT21"/>
     <mergeCell ref="S7:AD7"/>
@@ -5446,28 +5437,37 @@
     <mergeCell ref="Y17:AT17"/>
     <mergeCell ref="V8:X8"/>
     <mergeCell ref="S16:U16"/>
-    <mergeCell ref="S11:AT11"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:AT3"/>
-    <mergeCell ref="N4:R35"/>
-    <mergeCell ref="S4:AT4"/>
-    <mergeCell ref="S5:AT5"/>
-    <mergeCell ref="S6:AT6"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="AE16:AT16"/>
-    <mergeCell ref="AE18:AT18"/>
-    <mergeCell ref="S18:AD18"/>
-    <mergeCell ref="V9:AT9"/>
-    <mergeCell ref="T12:AT12"/>
-    <mergeCell ref="Y13:AT13"/>
-    <mergeCell ref="V14:AT14"/>
-    <mergeCell ref="S10:AT10"/>
+    <mergeCell ref="S22:U22"/>
+    <mergeCell ref="V22:X22"/>
+    <mergeCell ref="AE22:AT22"/>
+    <mergeCell ref="Y22:AA22"/>
+    <mergeCell ref="AB22:AD22"/>
+    <mergeCell ref="S23:U23"/>
+    <mergeCell ref="V23:X23"/>
+    <mergeCell ref="Y23:AT23"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="V24:X24"/>
+    <mergeCell ref="Y24:AT24"/>
+    <mergeCell ref="S25:U25"/>
+    <mergeCell ref="V25:X25"/>
+    <mergeCell ref="Y25:AA25"/>
+    <mergeCell ref="AB25:AT25"/>
+    <mergeCell ref="S26:U26"/>
+    <mergeCell ref="V26:X26"/>
+    <mergeCell ref="Y26:AA26"/>
+    <mergeCell ref="AB26:AT26"/>
+    <mergeCell ref="S29:U29"/>
+    <mergeCell ref="V29:X29"/>
+    <mergeCell ref="AE29:AT29"/>
+    <mergeCell ref="Y29:AD29"/>
+    <mergeCell ref="S27:U27"/>
+    <mergeCell ref="V27:X27"/>
+    <mergeCell ref="Y27:AA27"/>
+    <mergeCell ref="AB27:AT27"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="AE28:AT28"/>
+    <mergeCell ref="Y28:AD28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5477,8 +5477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84BD2F74-A48E-42CC-898E-3027680B67A9}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5488,37 +5488,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="74"/>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="G1" s="75" t="s">
+      <c r="A1" s="80"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="G1" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G2" s="80">
-        <v>0</v>
-      </c>
-      <c r="H2" s="80">
-        <v>0</v>
-      </c>
-      <c r="I2" s="80">
-        <v>0</v>
-      </c>
-      <c r="J2" s="80">
-        <v>0</v>
-      </c>
-      <c r="K2" s="80">
-        <v>0</v>
-      </c>
-      <c r="L2" s="80">
+      <c r="G2" s="54">
+        <v>0</v>
+      </c>
+      <c r="H2" s="54">
+        <v>0</v>
+      </c>
+      <c r="I2" s="54">
+        <v>0</v>
+      </c>
+      <c r="J2" s="54">
+        <v>0</v>
+      </c>
+      <c r="K2" s="54">
+        <v>0</v>
+      </c>
+      <c r="L2" s="54">
         <v>0</v>
       </c>
       <c r="M2" s="17" t="s">
@@ -5529,22 +5529,22 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G3" s="81">
-        <v>0</v>
-      </c>
-      <c r="H3" s="81">
-        <v>0</v>
-      </c>
-      <c r="I3" s="81">
-        <v>0</v>
-      </c>
-      <c r="J3" s="81">
-        <v>1</v>
-      </c>
-      <c r="K3" s="81">
-        <v>0</v>
-      </c>
-      <c r="L3" s="81">
+      <c r="G3" s="55">
+        <v>0</v>
+      </c>
+      <c r="H3" s="55">
+        <v>0</v>
+      </c>
+      <c r="I3" s="55">
+        <v>0</v>
+      </c>
+      <c r="J3" s="55">
+        <v>1</v>
+      </c>
+      <c r="K3" s="55">
+        <v>0</v>
+      </c>
+      <c r="L3" s="55">
         <v>0</v>
       </c>
       <c r="M3" s="13" t="s">
@@ -5555,25 +5555,25 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G4" s="80">
-        <v>0</v>
-      </c>
-      <c r="H4" s="80">
-        <v>0</v>
-      </c>
-      <c r="I4" s="80">
-        <v>1</v>
-      </c>
-      <c r="J4" s="80">
-        <v>0</v>
-      </c>
-      <c r="K4" s="80">
-        <v>0</v>
-      </c>
-      <c r="L4" s="80">
-        <v>0</v>
-      </c>
-      <c r="M4" s="83" t="s">
+      <c r="G4" s="54">
+        <v>0</v>
+      </c>
+      <c r="H4" s="54">
+        <v>0</v>
+      </c>
+      <c r="I4" s="54">
+        <v>1</v>
+      </c>
+      <c r="J4" s="54">
+        <v>0</v>
+      </c>
+      <c r="K4" s="54">
+        <v>0</v>
+      </c>
+      <c r="L4" s="54">
+        <v>0</v>
+      </c>
+      <c r="M4" s="57" t="s">
         <v>30</v>
       </c>
       <c r="N4" t="s">
@@ -5581,22 +5581,22 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G5" s="81">
-        <v>0</v>
-      </c>
-      <c r="H5" s="81">
-        <v>0</v>
-      </c>
-      <c r="I5" s="81">
-        <v>1</v>
-      </c>
-      <c r="J5" s="81">
-        <v>1</v>
-      </c>
-      <c r="K5" s="81">
-        <v>0</v>
-      </c>
-      <c r="L5" s="81">
+      <c r="G5" s="55">
+        <v>0</v>
+      </c>
+      <c r="H5" s="55">
+        <v>0</v>
+      </c>
+      <c r="I5" s="55">
+        <v>1</v>
+      </c>
+      <c r="J5" s="55">
+        <v>1</v>
+      </c>
+      <c r="K5" s="55">
+        <v>0</v>
+      </c>
+      <c r="L5" s="55">
         <v>0</v>
       </c>
       <c r="M5" s="13" t="s">
@@ -5607,305 +5607,304 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G6" s="80">
-        <v>0</v>
-      </c>
-      <c r="H6" s="80">
-        <v>1</v>
-      </c>
-      <c r="I6" s="80">
-        <v>0</v>
-      </c>
-      <c r="J6" s="80">
-        <v>0</v>
-      </c>
-      <c r="K6" s="80">
-        <v>0</v>
-      </c>
-      <c r="L6" s="80">
-        <v>0</v>
-      </c>
-      <c r="M6" s="83" t="s">
+      <c r="G6" s="54">
+        <v>0</v>
+      </c>
+      <c r="H6" s="54">
+        <v>1</v>
+      </c>
+      <c r="I6" s="54">
+        <v>0</v>
+      </c>
+      <c r="J6" s="54">
+        <v>0</v>
+      </c>
+      <c r="K6" s="54">
+        <v>0</v>
+      </c>
+      <c r="L6" s="54">
+        <v>0</v>
+      </c>
+      <c r="M6" s="57" t="s">
         <v>32</v>
       </c>
       <c r="N6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G7" s="81">
-        <v>0</v>
-      </c>
-      <c r="H7" s="81">
-        <v>1</v>
-      </c>
-      <c r="I7" s="81">
-        <v>0</v>
-      </c>
-      <c r="J7" s="81">
-        <v>1</v>
-      </c>
-      <c r="K7" s="81">
-        <v>0</v>
-      </c>
-      <c r="L7" s="81">
-        <v>0</v>
-      </c>
-      <c r="M7" s="81"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G8" s="80">
-        <v>0</v>
-      </c>
-      <c r="H8" s="80">
-        <v>1</v>
-      </c>
-      <c r="I8" s="80">
-        <v>1</v>
-      </c>
-      <c r="J8" s="80">
-        <v>0</v>
-      </c>
-      <c r="K8" s="80">
-        <v>0</v>
-      </c>
-      <c r="L8" s="80">
-        <v>0</v>
-      </c>
-      <c r="M8" s="80"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G9" s="81">
-        <v>0</v>
-      </c>
-      <c r="H9" s="81">
-        <v>1</v>
-      </c>
-      <c r="I9" s="81">
-        <v>1</v>
-      </c>
-      <c r="J9" s="81">
-        <v>1</v>
-      </c>
-      <c r="K9" s="81">
-        <v>0</v>
-      </c>
-      <c r="L9" s="81">
-        <v>0</v>
-      </c>
-      <c r="M9" s="81"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G10" s="80">
-        <v>1</v>
-      </c>
-      <c r="H10" s="80">
-        <v>0</v>
-      </c>
-      <c r="I10" s="80">
-        <v>0</v>
-      </c>
-      <c r="J10" s="80">
-        <v>0</v>
-      </c>
-      <c r="K10" s="80">
-        <v>0</v>
-      </c>
-      <c r="L10" s="80">
-        <v>0</v>
-      </c>
-      <c r="M10" s="80"/>
+    <row r="7" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="55">
+        <v>0</v>
+      </c>
+      <c r="H7" s="55">
+        <v>1</v>
+      </c>
+      <c r="I7" s="55">
+        <v>0</v>
+      </c>
+      <c r="J7" s="55">
+        <v>1</v>
+      </c>
+      <c r="K7" s="55">
+        <v>0</v>
+      </c>
+      <c r="L7" s="55">
+        <v>0</v>
+      </c>
+      <c r="M7" s="36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="54">
+        <v>0</v>
+      </c>
+      <c r="H8" s="54">
+        <v>1</v>
+      </c>
+      <c r="I8" s="54">
+        <v>1</v>
+      </c>
+      <c r="J8" s="54">
+        <v>0</v>
+      </c>
+      <c r="K8" s="54">
+        <v>0</v>
+      </c>
+      <c r="L8" s="54">
+        <v>0</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="55">
+        <v>0</v>
+      </c>
+      <c r="H9" s="55">
+        <v>1</v>
+      </c>
+      <c r="I9" s="55">
+        <v>1</v>
+      </c>
+      <c r="J9" s="55">
+        <v>1</v>
+      </c>
+      <c r="K9" s="55">
+        <v>0</v>
+      </c>
+      <c r="L9" s="55">
+        <v>0</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="54">
+        <v>1</v>
+      </c>
+      <c r="H10" s="54">
+        <v>0</v>
+      </c>
+      <c r="I10" s="54">
+        <v>0</v>
+      </c>
+      <c r="J10" s="54">
+        <v>0</v>
+      </c>
+      <c r="K10" s="54">
+        <v>0</v>
+      </c>
+      <c r="L10" s="54">
+        <v>0</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="81">
-        <v>1</v>
-      </c>
-      <c r="H11" s="81">
-        <v>0</v>
-      </c>
-      <c r="I11" s="81">
-        <v>0</v>
-      </c>
-      <c r="J11" s="81">
-        <v>1</v>
-      </c>
-      <c r="K11" s="81">
-        <v>0</v>
-      </c>
-      <c r="L11" s="81">
-        <v>0</v>
-      </c>
-      <c r="M11" s="81"/>
+      <c r="G11" s="55">
+        <v>1</v>
+      </c>
+      <c r="H11" s="55">
+        <v>0</v>
+      </c>
+      <c r="I11" s="55">
+        <v>0</v>
+      </c>
+      <c r="J11" s="55">
+        <v>1</v>
+      </c>
+      <c r="K11" s="55">
+        <v>0</v>
+      </c>
+      <c r="L11" s="55">
+        <v>0</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="80">
-        <v>1</v>
-      </c>
-      <c r="H12" s="80">
-        <v>0</v>
-      </c>
-      <c r="I12" s="80">
-        <v>1</v>
-      </c>
-      <c r="J12" s="80">
-        <v>0</v>
-      </c>
-      <c r="K12" s="80">
-        <v>0</v>
-      </c>
-      <c r="L12" s="80">
-        <v>0</v>
-      </c>
-      <c r="M12" s="80"/>
-    </row>
-    <row r="13" spans="1:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="81">
-        <v>1</v>
-      </c>
-      <c r="H13" s="81">
-        <v>0</v>
-      </c>
-      <c r="I13" s="81">
-        <v>1</v>
-      </c>
-      <c r="J13" s="81">
-        <v>1</v>
-      </c>
-      <c r="K13" s="81">
-        <v>0</v>
-      </c>
-      <c r="L13" s="81">
-        <v>0</v>
-      </c>
-      <c r="M13" s="81"/>
+      <c r="G12" s="54">
+        <v>1</v>
+      </c>
+      <c r="H12" s="54">
+        <v>0</v>
+      </c>
+      <c r="I12" s="54">
+        <v>1</v>
+      </c>
+      <c r="J12" s="54">
+        <v>0</v>
+      </c>
+      <c r="K12" s="54">
+        <v>0</v>
+      </c>
+      <c r="L12" s="54">
+        <v>0</v>
+      </c>
+      <c r="M12" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="55">
+        <v>1</v>
+      </c>
+      <c r="H13" s="55">
+        <v>0</v>
+      </c>
+      <c r="I13" s="55">
+        <v>1</v>
+      </c>
+      <c r="J13" s="55">
+        <v>1</v>
+      </c>
+      <c r="K13" s="55">
+        <v>0</v>
+      </c>
+      <c r="L13" s="55">
+        <v>0</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G14" s="80">
-        <v>1</v>
-      </c>
-      <c r="H14" s="80">
-        <v>1</v>
-      </c>
-      <c r="I14" s="80">
-        <v>0</v>
-      </c>
-      <c r="J14" s="80">
-        <v>0</v>
-      </c>
-      <c r="K14" s="80">
-        <v>0</v>
-      </c>
-      <c r="L14" s="80">
-        <v>0</v>
-      </c>
-      <c r="M14" s="80"/>
+      <c r="G14" s="54">
+        <v>1</v>
+      </c>
+      <c r="H14" s="54">
+        <v>1</v>
+      </c>
+      <c r="I14" s="54">
+        <v>0</v>
+      </c>
+      <c r="J14" s="54">
+        <v>0</v>
+      </c>
+      <c r="K14" s="54">
+        <v>0</v>
+      </c>
+      <c r="L14" s="54">
+        <v>0</v>
+      </c>
+      <c r="M14" s="54"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G15" s="81">
-        <v>1</v>
-      </c>
-      <c r="H15" s="81">
-        <v>1</v>
-      </c>
-      <c r="I15" s="81">
-        <v>0</v>
-      </c>
-      <c r="J15" s="81">
-        <v>1</v>
-      </c>
-      <c r="K15" s="81">
-        <v>0</v>
-      </c>
-      <c r="L15" s="81">
-        <v>0</v>
-      </c>
-      <c r="M15" s="81"/>
+      <c r="G15" s="55">
+        <v>1</v>
+      </c>
+      <c r="H15" s="55">
+        <v>1</v>
+      </c>
+      <c r="I15" s="55">
+        <v>0</v>
+      </c>
+      <c r="J15" s="55">
+        <v>1</v>
+      </c>
+      <c r="K15" s="55">
+        <v>0</v>
+      </c>
+      <c r="L15" s="55">
+        <v>0</v>
+      </c>
+      <c r="M15" s="55"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G16" s="80">
-        <v>1</v>
-      </c>
-      <c r="H16" s="80">
-        <v>1</v>
-      </c>
-      <c r="I16" s="80">
-        <v>1</v>
-      </c>
-      <c r="J16" s="80">
-        <v>0</v>
-      </c>
-      <c r="K16" s="80">
-        <v>0</v>
-      </c>
-      <c r="L16" s="80">
-        <v>0</v>
-      </c>
-      <c r="M16" s="80"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="G17" s="82">
-        <v>1</v>
-      </c>
-      <c r="H17" s="82">
-        <v>1</v>
-      </c>
-      <c r="I17" s="82">
-        <v>1</v>
-      </c>
-      <c r="J17" s="82">
-        <v>1</v>
-      </c>
-      <c r="K17" s="82">
-        <v>0</v>
-      </c>
-      <c r="L17" s="82">
-        <v>0</v>
-      </c>
-      <c r="M17" s="82"/>
-    </row>
-    <row r="19" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="76" t="s">
+      <c r="G16" s="54">
+        <v>1</v>
+      </c>
+      <c r="H16" s="54">
+        <v>1</v>
+      </c>
+      <c r="I16" s="54">
+        <v>1</v>
+      </c>
+      <c r="J16" s="54">
+        <v>0</v>
+      </c>
+      <c r="K16" s="54">
+        <v>0</v>
+      </c>
+      <c r="L16" s="54">
+        <v>0</v>
+      </c>
+      <c r="M16" s="54"/>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G17" s="56">
+        <v>1</v>
+      </c>
+      <c r="H17" s="56">
+        <v>1</v>
+      </c>
+      <c r="I17" s="56">
+        <v>1</v>
+      </c>
+      <c r="J17" s="56">
+        <v>1</v>
+      </c>
+      <c r="K17" s="56">
+        <v>0</v>
+      </c>
+      <c r="L17" s="56">
+        <v>0</v>
+      </c>
+      <c r="M17" s="56"/>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G19" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-    </row>
-    <row r="20" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="78">
-        <v>0</v>
-      </c>
-      <c r="H20" s="78">
-        <v>0</v>
-      </c>
-      <c r="I20" s="78">
-        <v>0</v>
-      </c>
-      <c r="J20" s="78">
-        <v>0</v>
-      </c>
-      <c r="K20" s="78">
-        <v>0</v>
-      </c>
-      <c r="L20" s="78">
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+    </row>
+    <row r="20" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="52">
+        <v>0</v>
+      </c>
+      <c r="H20" s="52">
+        <v>0</v>
+      </c>
+      <c r="I20" s="52">
+        <v>0</v>
+      </c>
+      <c r="J20" s="52">
+        <v>0</v>
+      </c>
+      <c r="K20" s="52">
+        <v>0</v>
+      </c>
+      <c r="L20" s="52">
         <v>1</v>
       </c>
       <c r="M20" s="13" t="s">
@@ -5915,26 +5914,23 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="79">
-        <v>0</v>
-      </c>
-      <c r="H21" s="79">
-        <v>0</v>
-      </c>
-      <c r="I21" s="79">
-        <v>0</v>
-      </c>
-      <c r="J21" s="79">
-        <v>1</v>
-      </c>
-      <c r="K21" s="79">
-        <v>0</v>
-      </c>
-      <c r="L21" s="79">
+    <row r="21" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="53">
+        <v>0</v>
+      </c>
+      <c r="H21" s="53">
+        <v>0</v>
+      </c>
+      <c r="I21" s="53">
+        <v>0</v>
+      </c>
+      <c r="J21" s="53">
+        <v>1</v>
+      </c>
+      <c r="K21" s="53">
+        <v>0</v>
+      </c>
+      <c r="L21" s="53">
         <v>1</v>
       </c>
       <c r="M21" s="13" t="s">
@@ -5944,26 +5940,23 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="78">
-        <v>0</v>
-      </c>
-      <c r="H22" s="78">
-        <v>0</v>
-      </c>
-      <c r="I22" s="78">
-        <v>1</v>
-      </c>
-      <c r="J22" s="78">
-        <v>0</v>
-      </c>
-      <c r="K22" s="78">
-        <v>0</v>
-      </c>
-      <c r="L22" s="78">
+    <row r="22" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="52">
+        <v>0</v>
+      </c>
+      <c r="H22" s="52">
+        <v>0</v>
+      </c>
+      <c r="I22" s="52">
+        <v>1</v>
+      </c>
+      <c r="J22" s="52">
+        <v>0</v>
+      </c>
+      <c r="K22" s="52">
+        <v>0</v>
+      </c>
+      <c r="L22" s="52">
         <v>1</v>
       </c>
       <c r="M22" s="13" t="s">
@@ -5973,23 +5966,23 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G23" s="79">
-        <v>0</v>
-      </c>
-      <c r="H23" s="79">
-        <v>0</v>
-      </c>
-      <c r="I23" s="79">
-        <v>1</v>
-      </c>
-      <c r="J23" s="79">
-        <v>1</v>
-      </c>
-      <c r="K23" s="79">
-        <v>0</v>
-      </c>
-      <c r="L23" s="79">
+    <row r="23" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="53">
+        <v>0</v>
+      </c>
+      <c r="H23" s="53">
+        <v>0</v>
+      </c>
+      <c r="I23" s="53">
+        <v>1</v>
+      </c>
+      <c r="J23" s="53">
+        <v>1</v>
+      </c>
+      <c r="K23" s="53">
+        <v>0</v>
+      </c>
+      <c r="L23" s="53">
         <v>1</v>
       </c>
       <c r="M23" s="13" t="s">
@@ -5999,24 +5992,24 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E24" s="13"/>
-      <c r="G24" s="78">
-        <v>0</v>
-      </c>
-      <c r="H24" s="78">
-        <v>1</v>
-      </c>
-      <c r="I24" s="78">
-        <v>0</v>
-      </c>
-      <c r="J24" s="78">
-        <v>0</v>
-      </c>
-      <c r="K24" s="78">
-        <v>0</v>
-      </c>
-      <c r="L24" s="78">
+      <c r="G24" s="52">
+        <v>0</v>
+      </c>
+      <c r="H24" s="52">
+        <v>1</v>
+      </c>
+      <c r="I24" s="52">
+        <v>0</v>
+      </c>
+      <c r="J24" s="52">
+        <v>0</v>
+      </c>
+      <c r="K24" s="52">
+        <v>0</v>
+      </c>
+      <c r="L24" s="52">
         <v>1</v>
       </c>
       <c r="M24" s="13" t="s">
@@ -6026,23 +6019,23 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G25" s="79">
-        <v>0</v>
-      </c>
-      <c r="H25" s="79">
-        <v>1</v>
-      </c>
-      <c r="I25" s="79">
-        <v>0</v>
-      </c>
-      <c r="J25" s="79">
-        <v>1</v>
-      </c>
-      <c r="K25" s="79">
-        <v>0</v>
-      </c>
-      <c r="L25" s="79">
+    <row r="25" spans="5:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="53">
+        <v>0</v>
+      </c>
+      <c r="H25" s="53">
+        <v>1</v>
+      </c>
+      <c r="I25" s="53">
+        <v>0</v>
+      </c>
+      <c r="J25" s="53">
+        <v>1</v>
+      </c>
+      <c r="K25" s="53">
+        <v>0</v>
+      </c>
+      <c r="L25" s="53">
         <v>1</v>
       </c>
       <c r="M25" s="17" t="s">
@@ -6052,234 +6045,234 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="G26" s="78">
-        <v>0</v>
-      </c>
-      <c r="H26" s="78">
-        <v>1</v>
-      </c>
-      <c r="I26" s="78">
-        <v>1</v>
-      </c>
-      <c r="J26" s="78">
-        <v>0</v>
-      </c>
-      <c r="K26" s="78">
-        <v>0</v>
-      </c>
-      <c r="L26" s="78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="G27" s="79">
-        <v>0</v>
-      </c>
-      <c r="H27" s="79">
-        <v>1</v>
-      </c>
-      <c r="I27" s="79">
-        <v>1</v>
-      </c>
-      <c r="J27" s="79">
-        <v>1</v>
-      </c>
-      <c r="K27" s="79">
-        <v>0</v>
-      </c>
-      <c r="L27" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="G28" s="78">
-        <v>1</v>
-      </c>
-      <c r="H28" s="78">
-        <v>0</v>
-      </c>
-      <c r="I28" s="78">
-        <v>0</v>
-      </c>
-      <c r="J28" s="78">
-        <v>0</v>
-      </c>
-      <c r="K28" s="78">
-        <v>0</v>
-      </c>
-      <c r="L28" s="78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="G29" s="79">
-        <v>1</v>
-      </c>
-      <c r="H29" s="79">
-        <v>0</v>
-      </c>
-      <c r="I29" s="79">
-        <v>0</v>
-      </c>
-      <c r="J29" s="79">
-        <v>1</v>
-      </c>
-      <c r="K29" s="79">
-        <v>0</v>
-      </c>
-      <c r="L29" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="G30" s="78">
-        <v>1</v>
-      </c>
-      <c r="H30" s="78">
-        <v>0</v>
-      </c>
-      <c r="I30" s="78">
-        <v>1</v>
-      </c>
-      <c r="J30" s="78">
-        <v>0</v>
-      </c>
-      <c r="K30" s="78">
-        <v>0</v>
-      </c>
-      <c r="L30" s="78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="G31" s="79">
-        <v>1</v>
-      </c>
-      <c r="H31" s="79">
-        <v>0</v>
-      </c>
-      <c r="I31" s="79">
-        <v>1</v>
-      </c>
-      <c r="J31" s="79">
-        <v>1</v>
-      </c>
-      <c r="K31" s="79">
-        <v>0</v>
-      </c>
-      <c r="L31" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="G32" s="78">
-        <v>1</v>
-      </c>
-      <c r="H32" s="78">
-        <v>1</v>
-      </c>
-      <c r="I32" s="78">
-        <v>0</v>
-      </c>
-      <c r="J32" s="78">
-        <v>0</v>
-      </c>
-      <c r="K32" s="78">
-        <v>0</v>
-      </c>
-      <c r="L32" s="78">
+    <row r="26" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G26" s="52">
+        <v>0</v>
+      </c>
+      <c r="H26" s="52">
+        <v>1</v>
+      </c>
+      <c r="I26" s="52">
+        <v>1</v>
+      </c>
+      <c r="J26" s="52">
+        <v>0</v>
+      </c>
+      <c r="K26" s="52">
+        <v>0</v>
+      </c>
+      <c r="L26" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G27" s="53">
+        <v>0</v>
+      </c>
+      <c r="H27" s="53">
+        <v>1</v>
+      </c>
+      <c r="I27" s="53">
+        <v>1</v>
+      </c>
+      <c r="J27" s="53">
+        <v>1</v>
+      </c>
+      <c r="K27" s="53">
+        <v>0</v>
+      </c>
+      <c r="L27" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G28" s="52">
+        <v>1</v>
+      </c>
+      <c r="H28" s="52">
+        <v>0</v>
+      </c>
+      <c r="I28" s="52">
+        <v>0</v>
+      </c>
+      <c r="J28" s="52">
+        <v>0</v>
+      </c>
+      <c r="K28" s="52">
+        <v>0</v>
+      </c>
+      <c r="L28" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G29" s="53">
+        <v>1</v>
+      </c>
+      <c r="H29" s="53">
+        <v>0</v>
+      </c>
+      <c r="I29" s="53">
+        <v>0</v>
+      </c>
+      <c r="J29" s="53">
+        <v>1</v>
+      </c>
+      <c r="K29" s="53">
+        <v>0</v>
+      </c>
+      <c r="L29" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G30" s="52">
+        <v>1</v>
+      </c>
+      <c r="H30" s="52">
+        <v>0</v>
+      </c>
+      <c r="I30" s="52">
+        <v>1</v>
+      </c>
+      <c r="J30" s="52">
+        <v>0</v>
+      </c>
+      <c r="K30" s="52">
+        <v>0</v>
+      </c>
+      <c r="L30" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G31" s="53">
+        <v>1</v>
+      </c>
+      <c r="H31" s="53">
+        <v>0</v>
+      </c>
+      <c r="I31" s="53">
+        <v>1</v>
+      </c>
+      <c r="J31" s="53">
+        <v>1</v>
+      </c>
+      <c r="K31" s="53">
+        <v>0</v>
+      </c>
+      <c r="L31" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G32" s="52">
+        <v>1</v>
+      </c>
+      <c r="H32" s="52">
+        <v>1</v>
+      </c>
+      <c r="I32" s="52">
+        <v>0</v>
+      </c>
+      <c r="J32" s="52">
+        <v>0</v>
+      </c>
+      <c r="K32" s="52">
+        <v>0</v>
+      </c>
+      <c r="L32" s="52">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G33" s="79">
-        <v>1</v>
-      </c>
-      <c r="H33" s="79">
-        <v>1</v>
-      </c>
-      <c r="I33" s="79">
-        <v>0</v>
-      </c>
-      <c r="J33" s="79">
-        <v>1</v>
-      </c>
-      <c r="K33" s="79">
-        <v>0</v>
-      </c>
-      <c r="L33" s="79">
+      <c r="G33" s="53">
+        <v>1</v>
+      </c>
+      <c r="H33" s="53">
+        <v>1</v>
+      </c>
+      <c r="I33" s="53">
+        <v>0</v>
+      </c>
+      <c r="J33" s="53">
+        <v>1</v>
+      </c>
+      <c r="K33" s="53">
+        <v>0</v>
+      </c>
+      <c r="L33" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G34" s="78">
-        <v>1</v>
-      </c>
-      <c r="H34" s="78">
-        <v>1</v>
-      </c>
-      <c r="I34" s="78">
-        <v>1</v>
-      </c>
-      <c r="J34" s="78">
-        <v>0</v>
-      </c>
-      <c r="K34" s="78">
-        <v>0</v>
-      </c>
-      <c r="L34" s="78">
+      <c r="G34" s="52">
+        <v>1</v>
+      </c>
+      <c r="H34" s="52">
+        <v>1</v>
+      </c>
+      <c r="I34" s="52">
+        <v>1</v>
+      </c>
+      <c r="J34" s="52">
+        <v>0</v>
+      </c>
+      <c r="K34" s="52">
+        <v>0</v>
+      </c>
+      <c r="L34" s="52">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G35" s="79">
-        <v>1</v>
-      </c>
-      <c r="H35" s="79">
-        <v>1</v>
-      </c>
-      <c r="I35" s="79">
-        <v>1</v>
-      </c>
-      <c r="J35" s="79">
-        <v>1</v>
-      </c>
-      <c r="K35" s="79">
-        <v>0</v>
-      </c>
-      <c r="L35" s="79">
+      <c r="G35" s="53">
+        <v>1</v>
+      </c>
+      <c r="H35" s="53">
+        <v>1</v>
+      </c>
+      <c r="I35" s="53">
+        <v>1</v>
+      </c>
+      <c r="J35" s="53">
+        <v>1</v>
+      </c>
+      <c r="K35" s="53">
+        <v>0</v>
+      </c>
+      <c r="L35" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G36" s="76" t="s">
+      <c r="G36" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="77"/>
-      <c r="L36" s="77"/>
-      <c r="M36" s="77"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="83"/>
+      <c r="J36" s="83"/>
+      <c r="K36" s="83"/>
+      <c r="L36" s="83"/>
+      <c r="M36" s="83"/>
     </row>
     <row r="37" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G37" s="78">
-        <v>0</v>
-      </c>
-      <c r="H37" s="78">
-        <v>0</v>
-      </c>
-      <c r="I37" s="78">
-        <v>0</v>
-      </c>
-      <c r="J37" s="78">
-        <v>0</v>
-      </c>
-      <c r="K37" s="78">
-        <v>1</v>
-      </c>
-      <c r="L37" s="78">
+      <c r="G37" s="52">
+        <v>0</v>
+      </c>
+      <c r="H37" s="52">
+        <v>0</v>
+      </c>
+      <c r="I37" s="52">
+        <v>0</v>
+      </c>
+      <c r="J37" s="52">
+        <v>0</v>
+      </c>
+      <c r="K37" s="52">
+        <v>1</v>
+      </c>
+      <c r="L37" s="52">
         <v>0</v>
       </c>
       <c r="M37" s="14" t="s">
@@ -6290,22 +6283,22 @@
       </c>
     </row>
     <row r="38" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G38" s="79">
-        <v>0</v>
-      </c>
-      <c r="H38" s="79">
-        <v>0</v>
-      </c>
-      <c r="I38" s="79">
-        <v>0</v>
-      </c>
-      <c r="J38" s="79">
-        <v>1</v>
-      </c>
-      <c r="K38" s="79">
-        <v>1</v>
-      </c>
-      <c r="L38" s="79">
+      <c r="G38" s="53">
+        <v>0</v>
+      </c>
+      <c r="H38" s="53">
+        <v>0</v>
+      </c>
+      <c r="I38" s="53">
+        <v>0</v>
+      </c>
+      <c r="J38" s="53">
+        <v>1</v>
+      </c>
+      <c r="K38" s="53">
+        <v>1</v>
+      </c>
+      <c r="L38" s="53">
         <v>0</v>
       </c>
       <c r="M38" s="17" t="s">
@@ -6316,22 +6309,22 @@
       </c>
     </row>
     <row r="39" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G39" s="78">
-        <v>0</v>
-      </c>
-      <c r="H39" s="78">
-        <v>0</v>
-      </c>
-      <c r="I39" s="78">
-        <v>1</v>
-      </c>
-      <c r="J39" s="78">
-        <v>0</v>
-      </c>
-      <c r="K39" s="78">
-        <v>1</v>
-      </c>
-      <c r="L39" s="78">
+      <c r="G39" s="52">
+        <v>0</v>
+      </c>
+      <c r="H39" s="52">
+        <v>0</v>
+      </c>
+      <c r="I39" s="52">
+        <v>1</v>
+      </c>
+      <c r="J39" s="52">
+        <v>0</v>
+      </c>
+      <c r="K39" s="52">
+        <v>1</v>
+      </c>
+      <c r="L39" s="52">
         <v>0</v>
       </c>
       <c r="M39" s="13" t="s">
@@ -6342,22 +6335,22 @@
       </c>
     </row>
     <row r="40" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G40" s="79">
-        <v>0</v>
-      </c>
-      <c r="H40" s="79">
-        <v>0</v>
-      </c>
-      <c r="I40" s="79">
-        <v>1</v>
-      </c>
-      <c r="J40" s="79">
-        <v>1</v>
-      </c>
-      <c r="K40" s="79">
-        <v>1</v>
-      </c>
-      <c r="L40" s="79">
+      <c r="G40" s="53">
+        <v>0</v>
+      </c>
+      <c r="H40" s="53">
+        <v>0</v>
+      </c>
+      <c r="I40" s="53">
+        <v>1</v>
+      </c>
+      <c r="J40" s="53">
+        <v>1</v>
+      </c>
+      <c r="K40" s="53">
+        <v>1</v>
+      </c>
+      <c r="L40" s="53">
         <v>0</v>
       </c>
       <c r="M40" s="17" t="s">
@@ -6368,22 +6361,22 @@
       </c>
     </row>
     <row r="41" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G41" s="78">
-        <v>0</v>
-      </c>
-      <c r="H41" s="78">
-        <v>1</v>
-      </c>
-      <c r="I41" s="78">
-        <v>0</v>
-      </c>
-      <c r="J41" s="78">
-        <v>0</v>
-      </c>
-      <c r="K41" s="78">
-        <v>1</v>
-      </c>
-      <c r="L41" s="78">
+      <c r="G41" s="52">
+        <v>0</v>
+      </c>
+      <c r="H41" s="52">
+        <v>1</v>
+      </c>
+      <c r="I41" s="52">
+        <v>0</v>
+      </c>
+      <c r="J41" s="52">
+        <v>0</v>
+      </c>
+      <c r="K41" s="52">
+        <v>1</v>
+      </c>
+      <c r="L41" s="52">
         <v>0</v>
       </c>
       <c r="M41" s="17" t="s">
@@ -6394,22 +6387,22 @@
       </c>
     </row>
     <row r="42" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G42" s="79">
-        <v>0</v>
-      </c>
-      <c r="H42" s="79">
-        <v>1</v>
-      </c>
-      <c r="I42" s="79">
-        <v>0</v>
-      </c>
-      <c r="J42" s="79">
-        <v>1</v>
-      </c>
-      <c r="K42" s="79">
-        <v>1</v>
-      </c>
-      <c r="L42" s="79">
+      <c r="G42" s="53">
+        <v>0</v>
+      </c>
+      <c r="H42" s="53">
+        <v>1</v>
+      </c>
+      <c r="I42" s="53">
+        <v>0</v>
+      </c>
+      <c r="J42" s="53">
+        <v>1</v>
+      </c>
+      <c r="K42" s="53">
+        <v>1</v>
+      </c>
+      <c r="L42" s="53">
         <v>0</v>
       </c>
       <c r="M42" s="13" t="s">
@@ -6420,22 +6413,22 @@
       </c>
     </row>
     <row r="43" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G43" s="78">
-        <v>0</v>
-      </c>
-      <c r="H43" s="78">
-        <v>1</v>
-      </c>
-      <c r="I43" s="78">
-        <v>1</v>
-      </c>
-      <c r="J43" s="78">
-        <v>0</v>
-      </c>
-      <c r="K43" s="78">
-        <v>1</v>
-      </c>
-      <c r="L43" s="78">
+      <c r="G43" s="52">
+        <v>0</v>
+      </c>
+      <c r="H43" s="52">
+        <v>1</v>
+      </c>
+      <c r="I43" s="52">
+        <v>1</v>
+      </c>
+      <c r="J43" s="52">
+        <v>0</v>
+      </c>
+      <c r="K43" s="52">
+        <v>1</v>
+      </c>
+      <c r="L43" s="52">
         <v>0</v>
       </c>
       <c r="M43" s="13" t="s">
@@ -6443,22 +6436,22 @@
       </c>
     </row>
     <row r="44" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G44" s="79">
-        <v>0</v>
-      </c>
-      <c r="H44" s="79">
-        <v>1</v>
-      </c>
-      <c r="I44" s="79">
-        <v>1</v>
-      </c>
-      <c r="J44" s="79">
-        <v>1</v>
-      </c>
-      <c r="K44" s="79">
-        <v>1</v>
-      </c>
-      <c r="L44" s="79">
+      <c r="G44" s="53">
+        <v>0</v>
+      </c>
+      <c r="H44" s="53">
+        <v>1</v>
+      </c>
+      <c r="I44" s="53">
+        <v>1</v>
+      </c>
+      <c r="J44" s="53">
+        <v>1</v>
+      </c>
+      <c r="K44" s="53">
+        <v>1</v>
+      </c>
+      <c r="L44" s="53">
         <v>0</v>
       </c>
       <c r="M44" s="19" t="s">
@@ -6466,162 +6459,162 @@
       </c>
     </row>
     <row r="45" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G45" s="78">
-        <v>1</v>
-      </c>
-      <c r="H45" s="78">
-        <v>0</v>
-      </c>
-      <c r="I45" s="78">
-        <v>0</v>
-      </c>
-      <c r="J45" s="78">
-        <v>0</v>
-      </c>
-      <c r="K45" s="78">
-        <v>1</v>
-      </c>
-      <c r="L45" s="78">
+      <c r="G45" s="52">
+        <v>1</v>
+      </c>
+      <c r="H45" s="52">
+        <v>0</v>
+      </c>
+      <c r="I45" s="52">
+        <v>0</v>
+      </c>
+      <c r="J45" s="52">
+        <v>0</v>
+      </c>
+      <c r="K45" s="52">
+        <v>1</v>
+      </c>
+      <c r="L45" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G46" s="79">
-        <v>1</v>
-      </c>
-      <c r="H46" s="79">
-        <v>0</v>
-      </c>
-      <c r="I46" s="79">
-        <v>0</v>
-      </c>
-      <c r="J46" s="79">
-        <v>1</v>
-      </c>
-      <c r="K46" s="79">
-        <v>1</v>
-      </c>
-      <c r="L46" s="79">
+      <c r="G46" s="53">
+        <v>1</v>
+      </c>
+      <c r="H46" s="53">
+        <v>0</v>
+      </c>
+      <c r="I46" s="53">
+        <v>0</v>
+      </c>
+      <c r="J46" s="53">
+        <v>1</v>
+      </c>
+      <c r="K46" s="53">
+        <v>1</v>
+      </c>
+      <c r="L46" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G47" s="78">
-        <v>1</v>
-      </c>
-      <c r="H47" s="78">
-        <v>0</v>
-      </c>
-      <c r="I47" s="78">
-        <v>1</v>
-      </c>
-      <c r="J47" s="78">
-        <v>0</v>
-      </c>
-      <c r="K47" s="78">
-        <v>1</v>
-      </c>
-      <c r="L47" s="78">
+      <c r="G47" s="52">
+        <v>1</v>
+      </c>
+      <c r="H47" s="52">
+        <v>0</v>
+      </c>
+      <c r="I47" s="52">
+        <v>1</v>
+      </c>
+      <c r="J47" s="52">
+        <v>0</v>
+      </c>
+      <c r="K47" s="52">
+        <v>1</v>
+      </c>
+      <c r="L47" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G48" s="79">
-        <v>1</v>
-      </c>
-      <c r="H48" s="79">
-        <v>0</v>
-      </c>
-      <c r="I48" s="79">
-        <v>1</v>
-      </c>
-      <c r="J48" s="79">
-        <v>1</v>
-      </c>
-      <c r="K48" s="79">
-        <v>1</v>
-      </c>
-      <c r="L48" s="79">
+      <c r="G48" s="53">
+        <v>1</v>
+      </c>
+      <c r="H48" s="53">
+        <v>0</v>
+      </c>
+      <c r="I48" s="53">
+        <v>1</v>
+      </c>
+      <c r="J48" s="53">
+        <v>1</v>
+      </c>
+      <c r="K48" s="53">
+        <v>1</v>
+      </c>
+      <c r="L48" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="G49" s="78">
-        <v>1</v>
-      </c>
-      <c r="H49" s="78">
-        <v>1</v>
-      </c>
-      <c r="I49" s="78">
-        <v>0</v>
-      </c>
-      <c r="J49" s="78">
-        <v>0</v>
-      </c>
-      <c r="K49" s="78">
-        <v>1</v>
-      </c>
-      <c r="L49" s="78">
+      <c r="G49" s="52">
+        <v>1</v>
+      </c>
+      <c r="H49" s="52">
+        <v>1</v>
+      </c>
+      <c r="I49" s="52">
+        <v>0</v>
+      </c>
+      <c r="J49" s="52">
+        <v>0</v>
+      </c>
+      <c r="K49" s="52">
+        <v>1</v>
+      </c>
+      <c r="L49" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="G50" s="79">
-        <v>1</v>
-      </c>
-      <c r="H50" s="79">
-        <v>1</v>
-      </c>
-      <c r="I50" s="79">
-        <v>0</v>
-      </c>
-      <c r="J50" s="79">
-        <v>1</v>
-      </c>
-      <c r="K50" s="79">
-        <v>1</v>
-      </c>
-      <c r="L50" s="79">
+      <c r="G50" s="53">
+        <v>1</v>
+      </c>
+      <c r="H50" s="53">
+        <v>1</v>
+      </c>
+      <c r="I50" s="53">
+        <v>0</v>
+      </c>
+      <c r="J50" s="53">
+        <v>1</v>
+      </c>
+      <c r="K50" s="53">
+        <v>1</v>
+      </c>
+      <c r="L50" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="G51" s="78">
-        <v>1</v>
-      </c>
-      <c r="H51" s="78">
-        <v>1</v>
-      </c>
-      <c r="I51" s="78">
-        <v>1</v>
-      </c>
-      <c r="J51" s="78">
-        <v>0</v>
-      </c>
-      <c r="K51" s="78">
-        <v>1</v>
-      </c>
-      <c r="L51" s="78">
+      <c r="G51" s="52">
+        <v>1</v>
+      </c>
+      <c r="H51" s="52">
+        <v>1</v>
+      </c>
+      <c r="I51" s="52">
+        <v>1</v>
+      </c>
+      <c r="J51" s="52">
+        <v>0</v>
+      </c>
+      <c r="K51" s="52">
+        <v>1</v>
+      </c>
+      <c r="L51" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="7:12" x14ac:dyDescent="0.3">
-      <c r="G52" s="79">
-        <v>1</v>
-      </c>
-      <c r="H52" s="79">
-        <v>1</v>
-      </c>
-      <c r="I52" s="79">
-        <v>1</v>
-      </c>
-      <c r="J52" s="79">
-        <v>1</v>
-      </c>
-      <c r="K52" s="79">
-        <v>1</v>
-      </c>
-      <c r="L52" s="79">
+      <c r="G52" s="53">
+        <v>1</v>
+      </c>
+      <c r="H52" s="53">
+        <v>1</v>
+      </c>
+      <c r="I52" s="53">
+        <v>1</v>
+      </c>
+      <c r="J52" s="53">
+        <v>1</v>
+      </c>
+      <c r="K52" s="53">
+        <v>1</v>
+      </c>
+      <c r="L52" s="53">
         <v>0</v>
       </c>
     </row>

</xml_diff>